<commit_message>
Support Basic Induction Machine C-Simulation. The IM has high magnetizing inductance so the desired bandwidth should be low or else the current loop regulation would fail and you cannot even get large high frequency ripples in your M-axis current.
</commit_message>
<xml_diff>
--- a/emachinery/jsons/ACMInfo.xlsx
+++ b/emachinery/jsons/ACMInfo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DrH\Codes\emachineryTestPYPI\emachinery\jsons\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58E03535-28C3-4F66-BF80-96E5B3360F77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66D95EE4-B986-4D7D-9390-03AC9077E459}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="27600" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="49">
   <si>
     <t>品牌</t>
   </si>
@@ -165,6 +165,9 @@
   </si>
   <si>
     <t>反伽马转子电阻 [Ohm]</t>
+  </si>
+  <si>
+    <t>母线电压 [Vdc]</t>
   </si>
 </sst>
 </file>
@@ -668,10 +671,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -842,144 +845,139 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="19">
-        <v>3200</v>
-      </c>
-      <c r="C9" s="19">
-        <v>3800</v>
-      </c>
-      <c r="D9" s="19">
-        <v>3200</v>
-      </c>
-      <c r="E9" s="19">
-        <v>3200</v>
-      </c>
-      <c r="F9" s="19">
-        <v>3000</v>
+      <c r="A9" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="18">
+        <v>48</v>
+      </c>
+      <c r="C9" s="18">
+        <v>48</v>
+      </c>
+      <c r="D9" s="18">
+        <v>48</v>
+      </c>
+      <c r="E9" s="18">
+        <v>24</v>
+      </c>
+      <c r="F9" s="18">
+        <v>600</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" s="19">
-        <v>0.7</v>
+        <v>3200</v>
       </c>
       <c r="C10" s="19">
-        <v>2.2400000000000002</v>
+        <v>3800</v>
       </c>
       <c r="D10" s="19">
-        <v>1.27</v>
+        <v>3200</v>
       </c>
       <c r="E10" s="19">
-        <v>0.13700000000000001</v>
+        <v>3200</v>
       </c>
       <c r="F10" s="19">
-        <f>F21</f>
-        <v>26.525824301130999</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="19">
+        <v>0.7</v>
+      </c>
+      <c r="C11" s="19">
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="D11" s="19">
+        <v>1.27</v>
+      </c>
+      <c r="E11" s="19">
+        <v>0.13700000000000001</v>
+      </c>
+      <c r="F11" s="19">
+        <f>F22</f>
+        <v>26.525824301130999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="19">
+      <c r="B12" s="19">
         <v>7</v>
       </c>
-      <c r="C11" s="19">
+      <c r="C12" s="19">
         <v>6.5</v>
       </c>
-      <c r="D11" s="19">
+      <c r="D12" s="19">
         <v>12.8</v>
       </c>
-      <c r="E11" s="19">
+      <c r="E12" s="19">
         <v>2.4</v>
       </c>
-      <c r="F11" s="19">
+      <c r="F12" s="19">
         <f>F7</f>
         <v>8.8000000000000007</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B12" s="19">
+      <c r="B13" s="19">
         <v>4.5</v>
       </c>
-      <c r="C12" s="19">
+      <c r="C13" s="19">
         <v>6.5</v>
       </c>
-      <c r="D12" s="19">
+      <c r="D13" s="19">
         <v>3</v>
       </c>
-      <c r="E12" s="19">
+      <c r="E13" s="19">
         <v>1.1000000000000001</v>
       </c>
-      <c r="F12" s="19">
-        <f>F11</f>
+      <c r="F13" s="19">
+        <f>F12</f>
         <v>8.8000000000000007</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B13" s="20"/>
-      <c r="C13" s="20"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="20">
-        <f>24.9</f>
-        <v>24.9</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B14" s="20"/>
       <c r="C14" s="20"/>
       <c r="D14" s="20"/>
       <c r="E14" s="20"/>
       <c r="F14" s="20">
-        <v>1.6</v>
+        <f>24.9</f>
+        <v>24.9</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B15" s="20">
-        <f t="shared" ref="B15:E16" si="0">B18/2</f>
-        <v>2.0499999999999998</v>
-      </c>
-      <c r="C15" s="20">
-        <f t="shared" si="0"/>
-        <v>0.7</v>
-      </c>
-      <c r="D15" s="20">
-        <f t="shared" si="0"/>
-        <v>0.46600000000000003</v>
-      </c>
-      <c r="E15" s="20">
-        <f t="shared" si="0"/>
-        <v>0.122</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="B15" s="20"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
       <c r="F15" s="20">
-        <f>(0.448+0.0249)*1000</f>
-        <v>472.9</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B16" s="20">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="B16:E17" si="0">B19/2</f>
         <v>2.0499999999999998</v>
       </c>
       <c r="C16" s="20">
@@ -1001,52 +999,56 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" s="20">
+        <f t="shared" si="0"/>
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="C17" s="20">
+        <f t="shared" si="0"/>
+        <v>0.7</v>
+      </c>
+      <c r="D17" s="20">
+        <f t="shared" si="0"/>
+        <v>0.46600000000000003</v>
+      </c>
+      <c r="E17" s="20">
+        <f t="shared" si="0"/>
+        <v>0.122</v>
+      </c>
+      <c r="F17" s="20">
+        <f>(0.448+0.0249)*1000</f>
+        <v>472.9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B17" s="20">
-        <f>B20/2</f>
+      <c r="B18" s="20">
+        <f>B21/2</f>
         <v>0.47499999999999998</v>
       </c>
-      <c r="C17" s="20">
-        <f t="shared" ref="C17:E17" si="1">C20/2</f>
+      <c r="C18" s="20">
+        <f t="shared" ref="C18:E18" si="1">C21/2</f>
         <v>0.2465</v>
       </c>
-      <c r="D17" s="20">
+      <c r="D18" s="20">
         <f t="shared" si="1"/>
         <v>0.152</v>
       </c>
-      <c r="E17" s="20">
+      <c r="E18" s="20">
         <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
-      <c r="F17" s="20">
+      <c r="F18" s="20">
         <v>3.04</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18" s="21">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="C18" s="21">
-        <v>1.4</v>
-      </c>
-      <c r="D18" s="21">
-        <v>0.93200000000000005</v>
-      </c>
-      <c r="E18" s="21">
-        <v>0.24399999999999999</v>
-      </c>
-      <c r="F18" s="21">
-        <f>2*F15</f>
-        <v>945.8</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B19" s="21">
         <v>4.0999999999999996</v>
@@ -1061,271 +1063,292 @@
         <v>0.24399999999999999</v>
       </c>
       <c r="F19" s="21">
-        <f t="shared" ref="F19:F20" si="2">2*F16</f>
+        <f>2*F16</f>
         <v>945.8</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" s="21">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="C20" s="21">
+        <v>1.4</v>
+      </c>
+      <c r="D20" s="21">
+        <v>0.93200000000000005</v>
+      </c>
+      <c r="E20" s="21">
+        <v>0.24399999999999999</v>
+      </c>
+      <c r="F20" s="21">
+        <f t="shared" ref="F20:F21" si="2">2*F17</f>
+        <v>945.8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="B20" s="21">
+      <c r="B21" s="21">
         <v>0.95</v>
       </c>
-      <c r="C20" s="21">
+      <c r="C21" s="21">
         <v>0.49299999999999999</v>
       </c>
-      <c r="D20" s="21">
+      <c r="D21" s="21">
         <v>0.30399999999999999</v>
       </c>
-      <c r="E20" s="21">
+      <c r="E21" s="21">
         <v>0.5</v>
       </c>
-      <c r="F20" s="21">
+      <c r="F21" s="21">
         <f t="shared" si="2"/>
         <v>6.08</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="14" t="s">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B21" s="21">
+      <c r="B22" s="21">
         <f>B5/(B6/60*2*3.1415926)</f>
         <v>0.31830989161357204</v>
       </c>
-      <c r="C21" s="21">
+      <c r="C22" s="21">
         <f>C5/(C6/60*2*3.1415926)</f>
         <v>0.63661978322714408</v>
       </c>
-      <c r="D21" s="21">
+      <c r="D22" s="21">
         <f>D5/(D6/60*2*3.1415926)</f>
         <v>1.2732395664542882</v>
       </c>
-      <c r="E21" s="21">
+      <c r="E22" s="21">
         <f>E5/(E6/60*2*3.1415926)</f>
         <v>0.13687325339383596</v>
       </c>
-      <c r="F21" s="21">
+      <c r="F22" s="21">
         <f>F5/(F6/60*2*3.1415926)</f>
         <v>26.525824301130999</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="13" t="s">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="22">
-        <f>B21/B7</f>
+      <c r="B23" s="22">
+        <f>B22/B7</f>
         <v>9.0945683318163439E-2</v>
       </c>
-      <c r="C22" s="22">
-        <f>C21/C7</f>
+      <c r="C23" s="22">
+        <f>C22/C7</f>
         <v>9.7941505111868318E-2</v>
       </c>
-      <c r="D22" s="22">
-        <f>D21/D7</f>
+      <c r="D23" s="22">
+        <f>D22/D7</f>
         <v>9.9471841129241262E-2</v>
       </c>
-      <c r="E22" s="22">
-        <f>E21/E7</f>
+      <c r="E23" s="22">
+        <f>E22/E7</f>
         <v>5.7030522247431652E-2</v>
       </c>
-      <c r="F22" s="22">
-        <f>F21/F7</f>
+      <c r="F23" s="22">
+        <f>F22/F7</f>
         <v>3.0142982160376133</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="7" t="s">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B23" s="23">
-        <f>B21/B7/1.414</f>
+      <c r="B24" s="23">
+        <f>B22/B7/1.414</f>
         <v>6.4318022148630444E-2</v>
       </c>
-      <c r="C23" s="23">
-        <f>C21/C7/1.414</f>
+      <c r="C24" s="23">
+        <f>C22/C7/1.414</f>
         <v>6.9265562313909707E-2</v>
       </c>
-      <c r="D23" s="23">
-        <f>D21/D7/1.414</f>
+      <c r="D24" s="23">
+        <f>D22/D7/1.414</f>
         <v>7.0347836725064547E-2</v>
       </c>
-      <c r="E23" s="23">
-        <f>E21/E7/1.414</f>
+      <c r="E24" s="23">
+        <f>E22/E7/1.414</f>
         <v>4.0332759722370333E-2</v>
       </c>
-      <c r="F23" s="23">
-        <f>F21/F7/1.414</f>
+      <c r="F24" s="23">
+        <f>F22/F7/1.414</f>
         <v>2.1317526280322583</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="13" t="s">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="B24" s="16">
-        <f>B23/1.5/B4</f>
+      <c r="B25" s="16">
+        <f>B24/1.5/B4</f>
         <v>1.0719670358105074E-2</v>
       </c>
-      <c r="C24" s="16">
-        <f>C23/1.5/C4</f>
+      <c r="C25" s="16">
+        <f>C24/1.5/C4</f>
         <v>1.1544260385651617E-2</v>
       </c>
-      <c r="D24" s="16">
-        <f>D23/1.5/D4</f>
+      <c r="D25" s="16">
+        <f>D24/1.5/D4</f>
         <v>1.1724639454177425E-2</v>
       </c>
-      <c r="E24" s="16">
-        <f>E23/1.5/E4</f>
+      <c r="E25" s="16">
+        <f>E24/1.5/E4</f>
         <v>2.6888506481580223E-2</v>
       </c>
-      <c r="F24" s="16">
-        <f>F23/1.5/F4</f>
+      <c r="F25" s="16">
+        <f>F24/1.5/F4</f>
         <v>0.71058420934408606</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="7" t="s">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B25" s="23">
-        <f>B23/1.5/B4*(1000/(1/B4/2/3.1415926*60))</f>
+      <c r="B26" s="23">
+        <f>B24/1.5/B4*(1000/(1/B4/2/3.1415926*60))</f>
         <v>4.4902449428616329</v>
       </c>
-      <c r="C25" s="23">
-        <f>C23/1.5/C4*(1000/(1/C4/2/3.1415926*60))</f>
+      <c r="C26" s="23">
+        <f>C24/1.5/C4*(1000/(1/C4/2/3.1415926*60))</f>
         <v>4.8356484000048354</v>
       </c>
-      <c r="D25" s="23">
-        <f>D23/1.5/D4*(1000/(1/D4/2/3.1415926*60))</f>
+      <c r="D26" s="23">
+        <f>D24/1.5/D4*(1000/(1/D4/2/3.1415926*60))</f>
         <v>4.9112054062549113</v>
       </c>
-      <c r="E25" s="23">
-        <f>E23/1.5/E4*(1000/(1/E4/2/3.1415926*60))</f>
+      <c r="E26" s="23">
+        <f>E24/1.5/E4*(1000/(1/E4/2/3.1415926*60))</f>
         <v>2.8157577662528155</v>
       </c>
-      <c r="F25" s="23">
-        <f>F23/1.5/F4*(1000/(1/F4/2/3.1415926*60))</f>
+      <c r="F26" s="23">
+        <f>F24/1.5/F4*(1000/(1/F4/2/3.1415926*60))</f>
         <v>148.82440625014877</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="7" t="s">
+    <row r="27" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B26" s="23">
-        <f>B25/1000*B6</f>
+      <c r="B27" s="23">
+        <f>B26/1000*B6</f>
         <v>13.470734828584897</v>
       </c>
-      <c r="C26" s="23">
-        <f>C25/1000*C6</f>
+      <c r="C27" s="23">
+        <f>C26/1000*C6</f>
         <v>14.506945200014506</v>
       </c>
-      <c r="D26" s="23">
-        <f>D25/1000*D6</f>
+      <c r="D27" s="23">
+        <f>D26/1000*D6</f>
         <v>14.733616218764736</v>
       </c>
-      <c r="E26" s="23">
-        <f>E25/1000*E6</f>
+      <c r="E27" s="23">
+        <f>E26/1000*E6</f>
         <v>8.4472732987584465</v>
       </c>
-      <c r="F26" s="23">
-        <f>F25/1000*F6</f>
+      <c r="F27" s="23">
+        <f>F26/1000*F6</f>
         <v>214.30714500021421</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="7" t="s">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B27" s="24">
-        <f t="shared" ref="B27" si="3">B26/1.414</f>
+      <c r="B28" s="24">
+        <f t="shared" ref="B28" si="3">B27/1.414</f>
         <v>9.5266865831576357</v>
       </c>
-      <c r="C27" s="24">
-        <f t="shared" ref="C27" si="4">C26/1.414</f>
+      <c r="C28" s="24">
+        <f t="shared" ref="C28" si="4">C27/1.414</f>
         <v>10.259508628015917</v>
       </c>
-      <c r="D27" s="24">
-        <f t="shared" ref="D27" si="5">D26/1.414</f>
+      <c r="D28" s="24">
+        <f t="shared" ref="D28" si="5">D27/1.414</f>
         <v>10.419813450328668</v>
       </c>
-      <c r="E27" s="24">
-        <f t="shared" ref="E27" si="6">E26/1.414</f>
+      <c r="E28" s="24">
+        <f t="shared" ref="E28" si="6">E27/1.414</f>
         <v>5.9740263781884346</v>
       </c>
-      <c r="F27" s="24">
-        <f t="shared" ref="F27" si="7">F26/1.414</f>
+      <c r="F28" s="24">
+        <f t="shared" ref="F28" si="7">F27/1.414</f>
         <v>151.56092291387145</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B28" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C28" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D28" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="E28" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="F28" s="10" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B29" s="10">
-        <v>10000</v>
-      </c>
-      <c r="C29" s="10">
-        <v>10000</v>
-      </c>
-      <c r="D29" s="10">
-        <v>10000</v>
-      </c>
-      <c r="E29" s="10">
-        <v>2000</v>
-      </c>
-      <c r="F29" s="10">
-        <v>10000</v>
+        <v>11</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F29" s="10" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B30" s="10">
+        <v>10000</v>
+      </c>
+      <c r="C30" s="10">
+        <v>10000</v>
+      </c>
+      <c r="D30" s="10">
+        <v>10000</v>
+      </c>
+      <c r="E30" s="10">
+        <v>2000</v>
+      </c>
+      <c r="F30" s="10">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B30" s="10">
+      <c r="B31" s="10">
         <v>2500</v>
       </c>
-      <c r="C30" s="10">
+      <c r="C31" s="10">
         <v>2500</v>
       </c>
-      <c r="D30" s="10">
+      <c r="D31" s="10">
         <v>2500</v>
       </c>
-      <c r="E30" s="10">
+      <c r="E31" s="10">
         <v>500</v>
       </c>
-      <c r="F30" s="10">
+      <c r="F31" s="10">
         <v>2500</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="15" t="s">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="F31" s="12" t="s">
+      <c r="F32" s="12" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[acmsimc] avoid compiling satlut.c; Marino2005 step by step debug (successfully add Gamma); Harnefors2005 does not work for NTU PM motor ACSM080-G02430LZ, but adding current derivative will make it work.
</commit_message>
<xml_diff>
--- a/emachinery/jsons/ACMInfo.xlsx
+++ b/emachinery/jsons/ACMInfo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DrH\Codes\emachineryTestPYPI\emachinery\jsons\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66D95EE4-B986-4D7D-9390-03AC9077E459}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B452223-E03E-4F99-B0DB-A35BD7B51572}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="27600" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="27600" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="基本参数" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="51">
   <si>
     <t>品牌</t>
   </si>
@@ -168,6 +168,12 @@
   </si>
   <si>
     <t>母线电压 [Vdc]</t>
+  </si>
+  <si>
+    <t>ACSM080-G02430LZ</t>
+  </si>
+  <si>
+    <t>18 slot, no skew</t>
   </si>
 </sst>
 </file>
@@ -283,7 +289,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -333,6 +339,9 @@
     <xf numFmtId="2" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -671,10 +680,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -683,9 +692,10 @@
     <col min="2" max="3" width="30.42578125" style="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27.5703125" style="12" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="21.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>22</v>
       </c>
@@ -704,8 +714,11 @@
       <c r="F1" s="11" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" s="25" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -723,7 +736,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -742,8 +755,11 @@
       <c r="F3" s="10" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>9</v>
       </c>
@@ -762,8 +778,11 @@
       <c r="F4" s="17">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" s="17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>2</v>
       </c>
@@ -782,8 +801,11 @@
       <c r="F5" s="17">
         <v>4000</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" s="17">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>3</v>
       </c>
@@ -802,8 +824,11 @@
       <c r="F6" s="17">
         <v>1440</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" s="17">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>5</v>
       </c>
@@ -822,8 +847,11 @@
       <c r="F7" s="17">
         <v>8.8000000000000007</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7" s="17">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>10</v>
       </c>
@@ -843,8 +871,11 @@
         <f>0.063*10000</f>
         <v>630</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8" s="18">
+        <v>16.2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>48</v>
       </c>
@@ -863,8 +894,11 @@
       <c r="F9" s="18">
         <v>600</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9" s="18">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>6</v>
       </c>
@@ -883,8 +917,11 @@
       <c r="F10" s="19">
         <v>3000</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10" s="19">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>7</v>
       </c>
@@ -904,8 +941,12 @@
         <f>F22</f>
         <v>26.525824301130999</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11" s="19">
+        <f>G22</f>
+        <v>2.3873241871017901</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>8</v>
       </c>
@@ -925,8 +966,12 @@
         <f>F7</f>
         <v>8.8000000000000007</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G12" s="19">
+        <f>G7</f>
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>41</v>
       </c>
@@ -946,8 +991,12 @@
         <f>F12</f>
         <v>8.8000000000000007</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G13" s="19">
+        <f>G12</f>
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>43</v>
       </c>
@@ -959,8 +1008,9 @@
         <f>24.9</f>
         <v>24.9</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G14" s="20"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>47</v>
       </c>
@@ -971,8 +1021,9 @@
       <c r="F15" s="20">
         <v>1.6</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G15" s="20"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>44</v>
       </c>
@@ -996,8 +1047,12 @@
         <f>(0.448+0.0249)*1000</f>
         <v>472.9</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G16" s="20">
+        <f>5.7</f>
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>45</v>
       </c>
@@ -1021,8 +1076,12 @@
         <f>(0.448+0.0249)*1000</f>
         <v>472.9</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G17" s="20">
+        <f>5.7</f>
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>42</v>
       </c>
@@ -1045,8 +1104,11 @@
       <c r="F18" s="20">
         <v>3.04</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G18" s="20">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
         <v>38</v>
       </c>
@@ -1066,8 +1128,12 @@
         <f>2*F16</f>
         <v>945.8</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G19" s="21">
+        <f>2*G16</f>
+        <v>11.4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
         <v>39</v>
       </c>
@@ -1084,11 +1150,15 @@
         <v>0.24399999999999999</v>
       </c>
       <c r="F20" s="21">
-        <f t="shared" ref="F20:F21" si="2">2*F17</f>
+        <f t="shared" ref="F20:G21" si="2">2*F17</f>
         <v>945.8</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G20" s="21">
+        <f t="shared" si="2"/>
+        <v>11.4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
         <v>40</v>
       </c>
@@ -1108,8 +1178,12 @@
         <f t="shared" si="2"/>
         <v>6.08</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G21" s="21">
+        <f t="shared" si="2"/>
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
         <v>4</v>
       </c>
@@ -1133,8 +1207,12 @@
         <f>F5/(F6/60*2*3.1415926)</f>
         <v>26.525824301130999</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G22" s="21">
+        <f>G5/(G6/60*2*3.1415926)</f>
+        <v>2.3873241871017901</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
         <v>21</v>
       </c>
@@ -1158,8 +1236,12 @@
         <f>F22/F7</f>
         <v>3.0142982160376133</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G23" s="22">
+        <f>G22/G7</f>
+        <v>0.56841052073852139</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>32</v>
       </c>
@@ -1183,8 +1265,12 @@
         <f>F22/F7/1.414</f>
         <v>2.1317526280322583</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G24" s="23">
+        <f>G22/G7/1.414</f>
+        <v>0.4019876384289402</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
         <v>46</v>
       </c>
@@ -1208,8 +1294,12 @@
         <f>F24/1.5/F4</f>
         <v>0.71058420934408606</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G25" s="16">
+        <f>G24/1.5/G4</f>
+        <v>6.6997939738156695E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>35</v>
       </c>
@@ -1233,8 +1323,12 @@
         <f>F24/1.5/F4*(1000/(1/F4/2/3.1415926*60))</f>
         <v>148.82440625014877</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G26" s="23">
+        <f>G24/1.5/G4*(1000/(1/G4/2/3.1415926*60))</f>
+        <v>28.064030892885199</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>36</v>
       </c>
@@ -1258,8 +1352,12 @@
         <f>F26/1000*F6</f>
         <v>214.30714500021421</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G27" s="23">
+        <f>G26/1000*G6</f>
+        <v>84.192092678655598</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>37</v>
       </c>
@@ -1280,11 +1378,15 @@
         <v>5.9740263781884346</v>
       </c>
       <c r="F28" s="24">
-        <f t="shared" ref="F28" si="7">F27/1.414</f>
+        <f t="shared" ref="F28:G28" si="7">F27/1.414</f>
         <v>151.56092291387145</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G28" s="24">
+        <f t="shared" si="7"/>
+        <v>59.541791144735221</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>11</v>
       </c>
@@ -1303,8 +1405,11 @@
       <c r="F29" s="10" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G29" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>12</v>
       </c>
@@ -1323,8 +1428,11 @@
       <c r="F30" s="10">
         <v>10000</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G30" s="10">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>13</v>
       </c>
@@ -1343,13 +1451,19 @@
       <c r="F31" s="10">
         <v>2500</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G31" s="10">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="15" t="s">
         <v>33</v>
       </c>
       <c r="F32" s="12" t="s">
         <v>34</v>
+      </c>
+      <c r="G32" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1360,18 +1474,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -1390,8 +1505,11 @@
       <c r="F1" s="11" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" s="25" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -1410,8 +1528,11 @@
       <c r="F2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
@@ -1430,8 +1551,11 @@
       <c r="F3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -1450,8 +1574,11 @@
       <c r="F4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
@@ -1470,8 +1597,11 @@
       <c r="F5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
@@ -1488,6 +1618,9 @@
         <v>0</v>
       </c>
       <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
         <v>0</v>
       </c>
     </row>

</xml_diff>